<commit_message>
LV_T1109_Contact_SelectionAndDeselectionOfSubscriptionPreferencesForExternalContact - Final - 22 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1109_Contact_SelectionAndDeselectionOfSubscriptionPreferencesForExternalContact.xlsx
+++ b/TestData/T1109_Contact_SelectionAndDeselectionOfSubscriptionPreferencesForExternalContact.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373A58EB-E88E-4B86-B995-B4E9752BF6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC8F323-49C9-4963-B015-16C51859F202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -407,18 +407,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -433,13 +433,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -456,13 +456,13 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -470,7 +470,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -510,7 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>